<commit_message>
vault backup: 2026-01-30 19:28:02
</commit_message>
<xml_diff>
--- a/utils/financial_modeling/luminous_wetland_monte_carlo_model.xlsx
+++ b/utils/financial_modeling/luminous_wetland_monte_carlo_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Luminous Dropbox/Obsidian/utils/financial_modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613CE668-89C2-F84E-BA78-222ABF5DA553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF63908-C207-6346-953A-07F6BEF4502D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Cover" sheetId="1" r:id="rId1"/>
@@ -3776,7 +3776,7 @@
   </sheetPr>
   <dimension ref="A1:I1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -34267,7 +34267,7 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -34949,7 +34949,7 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
vault backup: 2026-01-30 20:21:35
</commit_message>
<xml_diff>
--- a/utils/financial_modeling/luminous_wetland_monte_carlo_model.xlsx
+++ b/utils/financial_modeling/luminous_wetland_monte_carlo_model.xlsx
@@ -12170,7 +12170,11 @@
           <t>Active season length</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>6_Calc_Timeline, 9_Calc_Costs, 10_Calc_Sim</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">

</xml_diff>